<commit_message>
thesis + performance programs
</commit_message>
<xml_diff>
--- a/results/fibonacci.xlsx
+++ b/results/fibonacci.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mgr\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCBFCB2-DFFB-43A5-B103-AAF36EBB7FE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FB8AA1-CB4F-4699-8B6B-9FEEBAED4EBF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,13 +58,13 @@
     <t>original program</t>
   </si>
   <si>
-    <t>average for original program</t>
+    <t>x</t>
   </si>
   <si>
-    <t>average for interpreter</t>
+    <t>Average execution time of the original program</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Average execution time of the interpreter</t>
   </si>
 </sst>
 </file>
@@ -71,7 +72,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -112,19 +113,19 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -142,6 +143,1163 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>29.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F6F7-4BBC-8EF2-AEC9CB9ADC8C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F6F7-4BBC-8EF2-AEC9CB9ADC8C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>352.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>361.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>476.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1796.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15906.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>171231.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F6F7-4BBC-8EF2-AEC9CB9ADC8C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="88583455"/>
+        <c:axId val="195795295"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$3:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>35</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$A$3:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>35</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-F6F7-4BBC-8EF2-AEC9CB9ADC8C}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="88583455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="195795295"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="195795295"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="88583455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>214311</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66F465DD-E6FF-43D0-902F-F53329314030}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,457 +1565,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="17" style="2"/>
+    <col min="1" max="16384" width="17" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>28</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>29</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>29</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>31</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>32</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>346</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>327</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>328</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>373</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>388</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <f>AVERAGE(B3:F3)</f>
         <v>29.8</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="3">
         <f>AVERAGE(G3:K3)</f>
         <v>352.4</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="4">
         <f>M3/L3</f>
         <v>11.825503355704697</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>15</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>29</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>28</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>32</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>31</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>31</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>365</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>363</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>357</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>365</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>356</v>
       </c>
-      <c r="L4" s="4">
-        <f t="shared" ref="L4:L11" si="0">AVERAGE(B4:F4)</f>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L8" si="0">AVERAGE(B4:F4)</f>
         <v>30.2</v>
       </c>
-      <c r="M4" s="4">
-        <f t="shared" ref="M4:M11" si="1">AVERAGE(G4:K4)</f>
+      <c r="M4" s="3">
+        <f t="shared" ref="M4:M8" si="1">AVERAGE(G4:K4)</f>
         <v>361.2</v>
       </c>
-      <c r="N4" s="5">
-        <f t="shared" ref="N4:N11" si="2">M4/L4</f>
+      <c r="N4" s="4">
+        <f t="shared" ref="N4:N8" si="2">M4/L4</f>
         <v>11.960264900662251</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>20</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>30</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>29</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>30</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>31</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>29</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>467</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>488</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>480</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>478</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>468</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <f t="shared" si="0"/>
         <v>29.8</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <f t="shared" si="1"/>
         <v>476.2</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <f t="shared" si="2"/>
         <v>15.979865771812079</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>25</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>31</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>31</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>33</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>30</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>31</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>1690</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>1745</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>1869</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>1873</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>1805</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <f t="shared" si="0"/>
         <v>31.2</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="3">
         <f t="shared" si="1"/>
         <v>1796.4</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <f t="shared" si="2"/>
         <v>57.57692307692308</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>30</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>35</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>37</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>36</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>34</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>37</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>16375</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>15676</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>15433</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>16119</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>15931</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <f t="shared" si="0"/>
         <v>35.799999999999997</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <f t="shared" si="1"/>
         <v>15906.8</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <f t="shared" si="2"/>
         <v>444.32402234636874</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>35</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>94</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>93</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>97</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>94</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>91</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>173727</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>171936</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>169601</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>169510</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>171382</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <f t="shared" si="0"/>
         <v>93.8</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="3">
         <f t="shared" si="1"/>
         <v>171231.2</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="4">
         <f t="shared" si="2"/>
         <v>1825.4925373134331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>40</v>
-      </c>
-      <c r="B9" s="2">
-        <v>695</v>
-      </c>
-      <c r="C9" s="2">
-        <v>698</v>
-      </c>
-      <c r="D9" s="2">
-        <v>682</v>
-      </c>
-      <c r="E9" s="2">
-        <v>688</v>
-      </c>
-      <c r="F9" s="2">
-        <v>698</v>
-      </c>
-      <c r="L9" s="4">
-        <f t="shared" si="0"/>
-        <v>692.2</v>
-      </c>
-      <c r="M9" s="4" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N9" s="5" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>45</v>
-      </c>
-      <c r="B10" s="2">
-        <v>7418</v>
-      </c>
-      <c r="C10" s="2">
-        <v>7322</v>
-      </c>
-      <c r="D10" s="2">
-        <v>7384</v>
-      </c>
-      <c r="E10" s="2">
-        <v>7835</v>
-      </c>
-      <c r="F10" s="2">
-        <v>7492</v>
-      </c>
-      <c r="L10" s="4">
-        <f t="shared" si="0"/>
-        <v>7490.2</v>
-      </c>
-      <c r="M10" s="4" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N10" s="5" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>50</v>
-      </c>
-      <c r="B11" s="2">
-        <v>81685</v>
-      </c>
-      <c r="C11" s="2">
-        <v>81440</v>
-      </c>
-      <c r="D11" s="2">
-        <v>84010</v>
-      </c>
-      <c r="E11" s="2">
-        <v>84473</v>
-      </c>
-      <c r="F11" s="2">
-        <v>86852</v>
-      </c>
-      <c r="L11" s="4">
-        <f t="shared" si="0"/>
-        <v>83692</v>
-      </c>
-      <c r="M11" s="4" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" s="5" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -871,5 +1933,20 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29BE5FB-4985-4750-9D12-8A7D9FCEA4FB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y27" sqref="Y27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>